<commit_message>
add additional accounts (covid and others)
</commit_message>
<xml_diff>
--- a/simfin/federal/historical_accounts.xlsx
+++ b/simfin/federal/historical_accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliennavaux/Documents/simfin/simfin/federal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAC74F5-088B-DE4C-B9A1-9DABE66074BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CED9C4-41C4-0B49-A4A1-B1C77A1AA0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>account</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>other_transfers</t>
+  </si>
+  <si>
+    <t>additional_accounts</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,52 +514,52 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>4798</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>5539</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>7160</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>8028</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>8355</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>8552</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>7815</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>7391</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>7833</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>9286</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>9521</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>10030</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>11081</v>
       </c>
       <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1">
-        <v>8607</v>
-      </c>
-      <c r="S2" s="1">
-        <v>8951</v>
+        <v>11732</v>
+      </c>
+      <c r="R2">
+        <v>13124</v>
+      </c>
+      <c r="S2">
+        <v>13252</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -570,52 +573,52 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>4787</v>
+        <v>3185</v>
       </c>
       <c r="E3">
-        <v>4779</v>
+        <v>3649</v>
       </c>
       <c r="F3">
-        <v>4819</v>
+        <v>3925</v>
       </c>
       <c r="G3">
-        <v>4176</v>
+        <v>3740</v>
       </c>
       <c r="H3">
-        <v>3878</v>
+        <v>4148</v>
       </c>
       <c r="I3">
-        <v>3926</v>
+        <v>4309</v>
       </c>
       <c r="J3">
-        <v>4212</v>
+        <v>4511</v>
       </c>
       <c r="K3">
-        <v>4281</v>
+        <v>4792</v>
       </c>
       <c r="L3">
-        <v>3611</v>
+        <v>5290</v>
       </c>
       <c r="M3">
-        <v>3957</v>
+        <v>5282</v>
       </c>
       <c r="N3">
-        <v>5040</v>
+        <v>5487</v>
       </c>
       <c r="O3">
-        <v>5574</v>
+        <v>5946</v>
       </c>
       <c r="P3">
-        <v>6358</v>
+        <v>6096</v>
       </c>
       <c r="Q3">
-        <v>7457</v>
-      </c>
-      <c r="R3" s="1">
-        <v>6605</v>
-      </c>
-      <c r="S3" s="1">
-        <v>6702</v>
+        <v>6306</v>
+      </c>
+      <c r="R3">
+        <v>6617</v>
+      </c>
+      <c r="S3">
+        <v>6800</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -629,52 +632,111 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1209</v>
+        <v>3139</v>
       </c>
       <c r="E4">
-        <v>1391</v>
+        <v>2782</v>
       </c>
       <c r="F4">
-        <v>1440</v>
+        <v>3648</v>
       </c>
       <c r="G4">
-        <v>1630</v>
+        <v>3313</v>
       </c>
       <c r="H4">
-        <v>1617</v>
+        <v>4607</v>
       </c>
       <c r="I4">
-        <v>1847</v>
+        <v>4632</v>
       </c>
       <c r="J4">
-        <v>1747</v>
+        <v>4612</v>
       </c>
       <c r="K4">
-        <v>1753</v>
+        <v>5334</v>
       </c>
       <c r="L4">
-        <v>2014</v>
+        <v>5427</v>
       </c>
       <c r="M4">
-        <v>1880</v>
+        <v>3971</v>
       </c>
       <c r="N4">
-        <v>1976</v>
+        <v>3893</v>
       </c>
       <c r="O4">
-        <v>1906</v>
+        <v>4203</v>
       </c>
       <c r="P4">
-        <v>1784</v>
+        <v>5308</v>
       </c>
       <c r="Q4">
-        <v>1726</v>
-      </c>
-      <c r="R4" s="1">
-        <v>2002</v>
-      </c>
-      <c r="S4" s="1">
-        <v>2249</v>
+        <v>5082</v>
+      </c>
+      <c r="R4">
+        <v>5487</v>
+      </c>
+      <c r="S4">
+        <v>6625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>4039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>